<commit_message>
`Fixed model_id in handle_info_request function and updated differences_data filtering`
</commit_message>
<xml_diff>
--- a/output2.xlsx
+++ b/output2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="اطلاعات کلی"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="78">
   <si>
     <t>تفاوت ID</t>
   </si>
@@ -35,13 +35,46 @@
     <t>متن معرفی</t>
   </si>
   <si>
-    <t>دستگاه موپا برا یحکاکی دقیق روی فلزات</t>
-  </si>
-  <si>
-    <t>فایبر مناسب برای فلزات سنگین و متنوع</t>
-  </si>
-  <si>
-    <t>دیود برای مواد غیر فلزی مثل چوب و شیشه مناسب است</t>
+    <t>دستگاه موپا برا یحکاکی دقیق روی فلزات (موپا  دستی هوشمند)</t>
+  </si>
+  <si>
+    <t>دستگاه موپا برا یحکاکی دقیق روی فلزات (موپا میزدار هوشمند)</t>
+  </si>
+  <si>
+    <t>دستگاه موپا برا یحکاکی دقیق روی فلزات (موپا روی میز هوشمند)</t>
+  </si>
+  <si>
+    <t>فایبر مناسب برای فلزات سنگین و متنوع (فایبر دستی هوشمند)</t>
+  </si>
+  <si>
+    <t>فایبر مناسب برای فلزات سنگین و متنوع (فایبر میزدار هوشمند)</t>
+  </si>
+  <si>
+    <t>فایبر مناسب برای فلزات سنگین و متنوع (فایبر روی میز هوشمند)</t>
+  </si>
+  <si>
+    <t>فایبر مناسب برای فلزات سنگین و متنوع (فایبر دستی غیر هشمند)</t>
+  </si>
+  <si>
+    <t>فایبر مناسب برای فلزات سنگین و متنوع (فایبر میزدار غیر هوشمند)</t>
+  </si>
+  <si>
+    <t>فایبر مناسب برای فلزات سنگین و متنوع ( فایبر روی میز غیر هوشمند)</t>
+  </si>
+  <si>
+    <t>دیود برای مواد غیر فلزی مثل چوب و شیشه مناسب است (neje40w)</t>
+  </si>
+  <si>
+    <t>دیود برای مواد غیر فلزی مثل چوب و شیشه مناسب است (neje80w)</t>
+  </si>
+  <si>
+    <t>دیود برای مواد غیر فلزی مثل چوب و شیشه مناسب است (neje160w)</t>
+  </si>
+  <si>
+    <t>دیود برای مواد غیر فلزی مثل چوب و شیشه مناسب است(neje200w هوشمند)</t>
+  </si>
+  <si>
+    <t>دیود برای مواد غیر فلزی مثل چوب و شیشه مناسب است(neje200w باکس دار)</t>
   </si>
   <si>
     <t>ویژگی ID</t>
@@ -50,19 +83,46 @@
     <t>ویژگی ها</t>
   </si>
   <si>
-    <t>دقت بالا , حکاکی سریع</t>
-  </si>
-  <si>
-    <t>قابلیت تنظیم هوشمند,سرعت پردازش بالا</t>
-  </si>
-  <si>
-    <t>مناسب برای مواد غیر فلزی</t>
-  </si>
-  <si>
-    <t>سرعت برش بسیار بالا</t>
-  </si>
-  <si>
-    <t>باکس صنعتی و مناسب برای محیط های صنعتی</t>
+    <t>دقت بالا , حکاکی سریع (موپا دستی هوشمند)</t>
+  </si>
+  <si>
+    <t>دقت بالا , حکاکی سریع (موپا میزدار هوشمند)</t>
+  </si>
+  <si>
+    <t>دقت بالا , حکاکی سریع (موپا روی میز هوشمند)</t>
+  </si>
+  <si>
+    <t>قابلیت تنظیم هوشمند,سرعت پردازش بالا (فایبر دستی هوشمند)</t>
+  </si>
+  <si>
+    <t>قابلیت تنظیم هوشمند,سرعت پردازش بالا (فایبر میزدار هوشمند)</t>
+  </si>
+  <si>
+    <t>قابلیت تنظیم هوشمند,سرعت پردازش بالا (فایبر وی میز هوشمند)</t>
+  </si>
+  <si>
+    <t>مناسب برای مواد غیر فلزی (فایبر دستی غیر هوشمند)</t>
+  </si>
+  <si>
+    <t>مناسب برای مواد غیر فلزی (فایبر میزدار غیر هوشمند)</t>
+  </si>
+  <si>
+    <t>مناسب برای مواد غیر فلزی (فایبر روی میز غیر هوشمند)</t>
+  </si>
+  <si>
+    <t>سرعت برش بسیار بالا (40wneje)</t>
+  </si>
+  <si>
+    <t>سرعت برش بسیار بالا(neje80w)</t>
+  </si>
+  <si>
+    <t>سرعت برش بسیار بالا (neje160w)</t>
+  </si>
+  <si>
+    <t>باکس صنعتی و مناسب برای محیط های صنعتی(neje200 w)</t>
+  </si>
+  <si>
+    <t>باکس صنعتی و مناسب برای محیط های صنعتی(neje200w باکس دار)</t>
   </si>
   <si>
     <t>کاربرد ID</t>
@@ -586,7 +646,7 @@
   </sheetPr>
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -602,22 +662,22 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>15</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>3</v>
@@ -628,19 +688,19 @@
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F2" s="3">
         <v>1</v>
@@ -652,22 +712,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="3">
         <v>2</v>
@@ -676,22 +736,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>42</v>
+        <v>62</v>
       </c>
       <c r="F4" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G4" s="3">
         <v>3</v>
@@ -700,22 +760,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="4" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F5" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G5" s="3">
         <v>4</v>
@@ -726,22 +786,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="4" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F6" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G6" s="3">
         <v>5</v>
@@ -752,22 +812,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="4" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F7" s="3">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G7" s="3">
         <v>6</v>
@@ -778,22 +838,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F8" s="3">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G8" s="3">
         <v>7</v>
@@ -804,22 +864,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="4" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F9" s="3">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G9" s="3">
         <v>8</v>
@@ -830,22 +890,22 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="4" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>46</v>
+        <v>66</v>
       </c>
       <c r="F10" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G10" s="3">
         <v>9</v>
@@ -856,118 +916,118 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F11" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="G11" s="3">
         <v>10</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
       <c r="A12" s="4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F12" s="3">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G12" s="3">
         <v>11</v>
       </c>
       <c r="H12" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F13" s="3">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G13" s="3">
         <v>12</v>
       </c>
       <c r="H13" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F14" s="3">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="G14" s="3">
         <v>13</v>
       </c>
       <c r="H14" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="4" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="F15" s="3">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="G15" s="3">
         <v>14</v>
@@ -997,13 +1057,13 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
       <c r="A1" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
@@ -1011,10 +1071,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
@@ -1022,10 +1082,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -1033,10 +1093,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -1044,10 +1104,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
@@ -1055,10 +1115,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
@@ -1066,10 +1126,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
@@ -1077,10 +1137,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
@@ -1088,10 +1148,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
@@ -1099,10 +1159,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
@@ -1110,10 +1170,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
@@ -1121,10 +1181,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
@@ -1132,10 +1192,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
@@ -1143,10 +1203,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
@@ -1154,10 +1214,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1182,26 +1242,26 @@
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
@@ -1209,7 +1269,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
@@ -1217,7 +1277,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
@@ -1225,7 +1285,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
@@ -1233,7 +1293,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
@@ -1241,7 +1301,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
@@ -1249,7 +1309,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
@@ -1257,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
@@ -1265,7 +1325,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
@@ -1273,7 +1333,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>13</v>
+        <v>31</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
@@ -1281,7 +1341,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
@@ -1289,7 +1349,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
@@ -1297,7 +1357,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
@@ -1357,7 +1417,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
@@ -1365,7 +1425,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
@@ -1373,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
@@ -1381,7 +1441,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
@@ -1389,7 +1449,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
@@ -1397,7 +1457,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
@@ -1405,7 +1465,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
@@ -1413,7 +1473,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
@@ -1421,7 +1481,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
@@ -1429,7 +1489,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
@@ -1437,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
@@ -1445,7 +1505,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
@@ -1453,7 +1513,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1468,7 +1528,7 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>